<commit_message>
add react  4 components, for final output
</commit_message>
<xml_diff>
--- a/Comp230_excel.xlsx
+++ b/Comp230_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python101\rest APIs\comp230\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python101\rest APIs\comp240\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A6515-490C-4E00-9639-661579D4A44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE6F7FF-26D9-4A5B-904E-3AA691DA8747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E70C9E05-ABF2-4958-9103-533B18D641DA}"/>
+    <workbookView xWindow="-26985" yWindow="0" windowWidth="22365" windowHeight="16200" activeTab="2" xr2:uid="{E70C9E05-ABF2-4958-9103-533B18D641DA}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -269,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,7 +283,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B3A546-48AC-464A-9C4E-2499FF9D9B75}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,230 +611,229 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>2355</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>245</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>2566</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>2456</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>233</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1">
         <v>2541</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
         <v>2564</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>84562</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
         <v>6542</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>78452</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
         <v>521</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1">
         <v>123</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <v>654</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1">
         <v>85</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -866,10 +861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9397932-56E6-44F6-86E5-55EBB79E06C2}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,21 +875,18 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -905,7 +897,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -916,7 +908,7 @@
         <v>43856</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -927,7 +919,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -938,7 +930,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -949,7 +941,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -960,7 +952,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -971,7 +963,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -982,7 +974,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -993,7 +985,7 @@
         <v>43863</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1004,7 +996,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1015,7 +1007,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1026,7 +1018,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1037,7 +1029,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1048,7 +1040,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1067,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737FFFA6-984E-4617-95EB-3CFC44C638F5}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,16 +1076,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,14 +1507,6 @@
       <c r="D31" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1534,7 +1518,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,16 +1530,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1577,7 +1561,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1">
         <v>1.2</v>
@@ -1591,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1">
         <v>1.5</v>
@@ -1605,7 +1589,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1">
         <v>1.1000000000000001</v>
@@ -1619,7 +1603,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>1.3</v>
@@ -1633,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>1.9</v>
@@ -1647,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>1.5</v>
@@ -1661,7 +1645,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>1.6</v>
@@ -1675,7 +1659,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1">
         <v>1.4</v>
@@ -1689,7 +1673,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1">
         <v>1.33</v>
@@ -1703,7 +1687,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1">
         <v>1.5</v>
@@ -1717,7 +1701,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
         <v>1.6</v>
@@ -1731,7 +1715,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1">
         <v>1.4</v>
@@ -1745,7 +1729,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1">
         <v>1.33</v>
@@ -1759,7 +1743,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1">
         <v>1.4</v>

</xml_diff>

<commit_message>
table attempt to invoice app
</commit_message>
<xml_diff>
--- a/Comp230_excel.xlsx
+++ b/Comp230_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python101\rest APIs\comp240\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE6F7FF-26D9-4A5B-904E-3AA691DA8747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B18273F-7EB6-4E98-AA7A-7C8E7A4362E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="0" windowWidth="22365" windowHeight="16200" activeTab="2" xr2:uid="{E70C9E05-ABF2-4958-9103-533B18D641DA}"/>
+    <workbookView xWindow="30810" yWindow="1560" windowWidth="22365" windowHeight="13095" activeTab="1" xr2:uid="{E70C9E05-ABF2-4958-9103-533B18D641DA}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -863,15 +863,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9397932-56E6-44F6-86E5-55EBB79E06C2}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1061,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737FFFA6-984E-4617-95EB-3CFC44C638F5}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>